<commit_message>
The extra R-SQL ETL code is removed from HTN pdf and word tsd
</commit_message>
<xml_diff>
--- a/health_dimensions/supporting documents/HealthDimensions_NamingConvention.xlsx
+++ b/health_dimensions/supporting documents/HealthDimensions_NamingConvention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmcorg-my.sharepoint.com/personal/bill_adams_bmc_org/Documents/H2E_Dev/github_resources/h2edata/inst/resources/specifications/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shchakan\Documents\GitHub\PHX\health_dimensions\supporting documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{6C4F4F62-7A41-4F47-A4D2-E1015E8A88B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E34047D-B50A-45FB-B7C3-6066D263069F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40344489-113C-467F-B3EA-0C9DEBA73456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{8D42BCD2-B5A6-4F5B-9178-AFAFFA75E651}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D42BCD2-B5A6-4F5B-9178-AFAFFA75E651}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>COVID_02</t>
   </si>
   <si>
-    <t>covid_vaccination_ped_covid_02_tsd_01</t>
-  </si>
-  <si>
     <t>Diabetes Control</t>
   </si>
   <si>
@@ -227,18 +224,6 @@
     <t>BH_02</t>
   </si>
   <si>
-    <t>schizophrenia_c_icd_01_base</t>
-  </si>
-  <si>
-    <t>schizophrenia_c_icd_01</t>
-  </si>
-  <si>
-    <t>bipolar_c_icd_01_base</t>
-  </si>
-  <si>
-    <t>bipolar_c_icd_01</t>
-  </si>
-  <si>
     <t>Substance Use Disorder</t>
   </si>
   <si>
@@ -378,6 +363,21 @@
   </si>
   <si>
     <t>phq_any_01</t>
+  </si>
+  <si>
+    <t>covid_vaccinations_ped_covid_02_tsd_01</t>
+  </si>
+  <si>
+    <t>schizophrenia_01_base</t>
+  </si>
+  <si>
+    <t>schizophrenia_01</t>
+  </si>
+  <si>
+    <t>bipolar_01_base</t>
+  </si>
+  <si>
+    <t>bipolar_01</t>
   </si>
 </sst>
 </file>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D31E6E2-4865-478A-A515-6037B90691CE}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,61 +832,61 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>21</v>
@@ -942,259 +942,259 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E34" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E39" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E40" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E41" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E45" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E48" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>